<commit_message>
outside table definition sheet and update table definition
</commit_message>
<xml_diff>
--- a/02_詳細設計書/詳細設計書.xlsx
+++ b/02_詳細設計書/詳細設計書.xlsx
@@ -4,21 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="45" windowWidth="19395" windowHeight="7155" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="45" windowWidth="19395" windowHeight="7155" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="詳細設計書" sheetId="1" r:id="rId1"/>
     <sheet name="処理フロー" sheetId="4" r:id="rId2"/>
     <sheet name="メッセージ定義" sheetId="5" r:id="rId3"/>
     <sheet name="ログ定義" sheetId="6" r:id="rId4"/>
-    <sheet name="テーブル定義" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="71">
   <si>
     <t>起動方法</t>
     <rPh sb="0" eb="2">
@@ -609,179 +608,6 @@
   </si>
   <si>
     <t>ログメッセージ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テーブル名</t>
-    <rPh sb="4" eb="5">
-      <t>メイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テーブル情報</t>
-    <rPh sb="4" eb="6">
-      <t>ジョウホウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>カラム名</t>
-    <rPh sb="3" eb="4">
-      <t>メイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>型</t>
-    <rPh sb="0" eb="1">
-      <t>カタ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>桁数</t>
-    <rPh sb="0" eb="2">
-      <t>ケタスウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>フォーマット</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>制約</t>
-    <rPh sb="0" eb="2">
-      <t>セイヤク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>user_id</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>user_name</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>password</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>serial</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>character</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>000</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>FK</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>NOTNULL</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>WorkManage</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>startTime</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>endTime</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>HH:mm</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>workingTime</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>contents</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>note</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>worktime</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>uptime</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>deleteFlg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>updateFlg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>insertFlg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0/1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>integer</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>timestamp</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>yyyy/MM/dd</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>デフォルト書式</t>
-    <rPh sb="5" eb="7">
-      <t>ショシキ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PK</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>role</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>User_role</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Users</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -891,7 +717,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -911,12 +737,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1349,8 +1169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1464,10 +1284,10 @@
         <v>18</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>105</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.15">
@@ -1550,7 +1370,7 @@
         <v>19</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>107</v>
+        <v>69</v>
       </c>
       <c r="E21" s="3"/>
     </row>
@@ -1562,7 +1382,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="E22" s="3"/>
     </row>
@@ -1586,7 +1406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1658,382 +1478,4 @@
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G28"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="2" max="2" width="12.375" customWidth="1"/>
-    <col min="3" max="3" width="9.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:7" ht="18.75" x14ac:dyDescent="0.15">
-      <c r="B2" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C6" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E6" s="3">
-        <v>100</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E7" s="3">
-        <v>20</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C8" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="3">
-        <v>20</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B11" t="s">
-        <v>67</v>
-      </c>
-      <c r="C11" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C13" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E13" s="3">
-        <v>100</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C14" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E14" s="3">
-        <v>5</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="B17" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C18" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E18" s="3">
-        <v>100</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C19" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E19" s="3">
-        <v>5</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C20" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="3">
-        <v>5</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C21" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="3">
-        <v>5</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C22" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E22" s="3">
-        <v>20</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C23" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E23" s="3">
-        <v>20</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C24" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C25" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C26" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E26" s="3">
-        <v>1</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C27" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E27" s="3">
-        <v>1</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.15">
-      <c r="C28" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E28" s="3">
-        <v>1</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>